<commit_message>
Working about computer page
</commit_message>
<xml_diff>
--- a/green500_top_201611(edited).xlsx
+++ b/green500_top_201611(edited).xlsx
@@ -1327,7 +1327,7 @@
     <t xml:space="preserve">AMD x86_64</t>
   </si>
   <si>
-    <t xml:space="preserve">Opteron 6200 Series "Interlagos"</t>
+    <t xml:space="preserve">Opteron 6200 Series - Interlagos</t>
   </si>
   <si>
     <t xml:space="preserve">Cray XK7 </t>
@@ -2092,7 +2092,7 @@
     <t xml:space="preserve">HP Apollo 6000 Xl230/250 </t>
   </si>
   <si>
-    <t xml:space="preserve">Supercomputer System for Statistical Science "I"</t>
+    <t xml:space="preserve">Supercomputer System for Statistical Science</t>
   </si>
   <si>
     <t xml:space="preserve">SGI ICE X, Intel Xeon E5-2697v2/E5-2680v3 12C/12C 2.7GHz/2.5GHz, Infiniband FDR, Intel Xeon Phi 5120D</t>
@@ -3259,7 +3259,7 @@
     <t xml:space="preserve">Opteron 6344 12C 2.6GHz</t>
   </si>
   <si>
-    <t xml:space="preserve">Opteron 6300 Series "Abu Dhabi"</t>
+    <t xml:space="preserve">Opteron 6300 Series - Abu Dhabi</t>
   </si>
   <si>
     <t xml:space="preserve">Intel SC D2P4</t>
@@ -3424,7 +3424,7 @@
     <t xml:space="preserve">SuperMicro Twin^2, Xeon E5-2680v3 12C 2.5GHz, Infiniband FDR, NVIDIA Tesla K80</t>
   </si>
   <si>
-    <t xml:space="preserve">National Research Centre "Kurchatov Institute"</t>
+    <t xml:space="preserve">National Research Centre - Kurchatov Institute</t>
   </si>
   <si>
     <t xml:space="preserve">SuperMicro/Mellanox</t>
@@ -3556,7 +3556,7 @@
     <t xml:space="preserve">Opteron 6136 8C 2.4GHz</t>
   </si>
   <si>
-    <t xml:space="preserve">Opteron 6100-series "Magny-Cours" </t>
+    <t xml:space="preserve">Opteron 6100 Series - Magny-Cours</t>
   </si>
   <si>
     <t xml:space="preserve">Lenovo ThinkServer RD650, Xeon E5-2650v3 10C 2GHz, 10G Ethernet</t>
@@ -3948,24 +3948,28 @@
   </sheetPr>
   <dimension ref="A1:AJ501"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB6" activeCellId="0" sqref="AB6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AD76" activeCellId="0" sqref="AD76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="104.214285714286"/>
-    <col collapsed="false" hidden="false" max="18" min="8" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="27" min="25" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="36" min="29" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.1275510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="101.785714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="65.5765306122449"/>
+    <col collapsed="false" hidden="false" max="19" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="27" min="25" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="36" min="31" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>